<commit_message>
Updated excel example for better testing.
</commit_message>
<xml_diff>
--- a/src/test/resources/example1.xlsx
+++ b/src/test/resources/example1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Popis</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Hodnota</t>
   </si>
@@ -403,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G7:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,25 +413,22 @@
   </cols>
   <sheetData>
     <row r="7" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
       <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
         <v>3</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>4</v>
-      </c>
-      <c r="K7" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>10</v>
@@ -451,7 +445,7 @@
     </row>
     <row r="9" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="4">
         <v>10.5</v>
@@ -462,7 +456,7 @@
     </row>
     <row r="10" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
         <f>SUM(H8,H9)</f>
@@ -491,26 +485,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>